<commit_message>
Added  Page classes for requests
</commit_message>
<xml_diff>
--- a/resources/DATAFILE.xlsx
+++ b/resources/DATAFILE.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://amedeloitte-my.sharepoint.com/personal/chaidb_deloitte_com/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\makzarak\Desktop\Bench\Framework\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BE9EA091-604A-4FE6-A53D-052C6A445516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A1816C2-0C98-41F6-B34C-A9DDD3BE3758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5F3B00A6-1F83-4E01-BEDD-A24AF5294CA6}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{5F3B00A6-1F83-4E01-BEDD-A24AF5294CA6}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA_FILE" sheetId="1" r:id="rId1"/>
+    <sheet name="API_DATA_FILE" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="40">
   <si>
     <t>TC_NAME</t>
   </si>
@@ -142,6 +143,18 @@
   </si>
   <si>
     <t>Powerbank</t>
+  </si>
+  <si>
+    <t>TC_001_POST_SINGLE_USER</t>
+  </si>
+  <si>
+    <t>JOB</t>
+  </si>
+  <si>
+    <t>Developer</t>
+  </si>
+  <si>
+    <t>Ak</t>
   </si>
 </sst>
 </file>
@@ -515,25 +528,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D199509-3F83-478C-9D52-DA2EDFB81A9C}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection sqref="A1:J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="33.44140625" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" customWidth="1"/>
-    <col min="6" max="6" width="23.109375" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" customWidth="1"/>
+    <col min="1" max="1" width="33.453125" customWidth="1"/>
+    <col min="2" max="2" width="16.54296875" customWidth="1"/>
+    <col min="3" max="3" width="14.6328125" customWidth="1"/>
+    <col min="4" max="4" width="16.08984375" customWidth="1"/>
+    <col min="5" max="5" width="12.6328125" customWidth="1"/>
+    <col min="6" max="6" width="23.08984375" customWidth="1"/>
+    <col min="7" max="7" width="9.6328125" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
-    <col min="9" max="9" width="17.6640625" customWidth="1"/>
+    <col min="9" max="9" width="17.6328125" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -566,7 +579,7 @@
       </c>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -589,7 +602,7 @@
         <v>7349017534</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -606,7 +619,7 @@
         <v>7349017534</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -620,7 +633,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -634,7 +647,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -648,7 +661,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -656,7 +669,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -676,7 +689,7 @@
         <v>9731749971</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -684,7 +697,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -692,7 +705,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -700,7 +713,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -708,7 +721,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -716,7 +729,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -724,7 +737,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -732,7 +745,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -759,7 +772,96 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05C89F5F-990D-45BE-B25B-C73F98D7172B}">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="27.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C3" s="2"/>
+      <c r="E3" s="2"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="supriya@36" xr:uid="{B9E959BB-1A85-457C-B468-E85F1FA51C03}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100066650AE11F9D94F9BEC415F2F7F71AC" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="39d218c5b218fd11c7b1e015428ba1b0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8f0c852b-215b-4ad8-8d40-2e4064e0668d" xmlns:ns4="9c6c6072-304f-419a-b7e8-c670f973c5eb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e32445469b0a8b73f6a34ac0168539e2" ns3:_="" ns4:_="">
     <xsd:import namespace="8f0c852b-215b-4ad8-8d40-2e4064e0668d"/>
@@ -956,22 +1058,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC7F54BF-14C3-4105-920F-7FCBFFA7E40D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="8f0c852b-215b-4ad8-8d40-2e4064e0668d"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="9c6c6072-304f-419a-b7e8-c670f973c5eb"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5040F04D-8C74-4CDD-9A06-087701F18320}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9838879D-783C-41A7-8468-DC0782555013}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -988,29 +1100,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5040F04D-8C74-4CDD-9A06-087701F18320}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC7F54BF-14C3-4105-920F-7FCBFFA7E40D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="8f0c852b-215b-4ad8-8d40-2e4064e0668d"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="9c6c6072-304f-419a-b7e8-c670f973c5eb"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Pull request to merge ui and api
</commit_message>
<xml_diff>
--- a/resources/DATAFILE.xlsx
+++ b/resources/DATAFILE.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My Learning\Framework\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\makzarak\Desktop\example\Framework\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{703B4836-EED8-4F1E-9FF5-9790FA9EEB60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F262CABF-15DC-4262-8C7D-EFEFF22568DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5F3B00A6-1F83-4E01-BEDD-A24AF5294CA6}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{5F3B00A6-1F83-4E01-BEDD-A24AF5294CA6}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA_FILE" sheetId="1" r:id="rId1"/>
+    <sheet name="API_DATA_FILE" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="46">
   <si>
     <t>TC_NAME</t>
   </si>
@@ -142,13 +143,43 @@
   </si>
   <si>
     <t>TC_002_AMAZON_LOGIN</t>
+  </si>
+  <si>
+    <t>JOB</t>
+  </si>
+  <si>
+    <t>COUNTRY</t>
+  </si>
+  <si>
+    <t>STATE</t>
+  </si>
+  <si>
+    <t>CITY</t>
+  </si>
+  <si>
+    <t>TC_001_POST_SINGLE_USER</t>
+  </si>
+  <si>
+    <t>Ak</t>
+  </si>
+  <si>
+    <t>Developer</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>KN</t>
+  </si>
+  <si>
+    <t>Bengaluru</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,6 +203,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -181,7 +220,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -189,15 +228,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF616161"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF616161"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF616161"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF616161"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -515,7 +581,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D199509-3F83-478C-9D52-DA2EDFB81A9C}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -759,13 +825,76 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AC01BA1-7E02-4B9A-B53C-B29C9722552F}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="A1:F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="36.26953125" customWidth="1"/>
+    <col min="3" max="3" width="30.26953125" customWidth="1"/>
+    <col min="4" max="4" width="25.54296875" customWidth="1"/>
+    <col min="5" max="5" width="15.54296875" customWidth="1"/>
+    <col min="6" max="6" width="37.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" tooltip="mailto:supriya@36" display="mailto:supriya@36" xr:uid="{1B13A03D-8BC4-41AA-91A4-F03A00E03031}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -966,15 +1095,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5040F04D-8C74-4CDD-9A06-087701F18320}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC7F54BF-14C3-4105-920F-7FCBFFA7E40D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="8f0c852b-215b-4ad8-8d40-2e4064e0668d"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="9c6c6072-304f-419a-b7e8-c670f973c5eb"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -999,18 +1140,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC7F54BF-14C3-4105-920F-7FCBFFA7E40D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5040F04D-8C74-4CDD-9A06-087701F18320}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="8f0c852b-215b-4ad8-8d40-2e4064e0668d"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="9c6c6072-304f-419a-b7e8-c670f973c5eb"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Modified DATAFILE and RUNNERFILE to include API TESTCASES
</commit_message>
<xml_diff>
--- a/resources/DATAFILE.xlsx
+++ b/resources/DATAFILE.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\makzarak\Desktop\example\Framework\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My Learning\Framework\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F262CABF-15DC-4262-8C7D-EFEFF22568DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5102854C-E6AD-4780-95C4-928A409F695C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{5F3B00A6-1F83-4E01-BEDD-A24AF5294CA6}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="60">
   <si>
     <t>TC_NAME</t>
   </si>
@@ -173,13 +173,55 @@
   </si>
   <si>
     <t>Bengaluru</t>
+  </si>
+  <si>
+    <t>TC_002_LOGIN_TEST</t>
+  </si>
+  <si>
+    <t>TC_001_LOGIN_TEST_1</t>
+  </si>
+  <si>
+    <t>TC_002_LOGIN_TEST_2</t>
+  </si>
+  <si>
+    <t>TC_003_LOGIN_TEST_3</t>
+  </si>
+  <si>
+    <t>TC_002_HOMEPAGE_TEST_2</t>
+  </si>
+  <si>
+    <t>TC_003_HOMEPAGE_TEST_3</t>
+  </si>
+  <si>
+    <t>TC_001_INVENTORY_TEST_1</t>
+  </si>
+  <si>
+    <t>Edge</t>
+  </si>
+  <si>
+    <t>TC_002_INVENTORY_TEST_2</t>
+  </si>
+  <si>
+    <t>TC_003_INVENTORY_TEST_3</t>
+  </si>
+  <si>
+    <t>TC_002_HOMEPAGE_TEST_1</t>
+  </si>
+  <si>
+    <t>TC_002_HOMEPAGE_TEST_3</t>
+  </si>
+  <si>
+    <t>TC_002_HOMEPAGE_TEST_4</t>
+  </si>
+  <si>
+    <t>TC_002_HOMEPAGE_TEST_5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -211,6 +253,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -220,7 +269,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -228,40 +277,26 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF616161"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF616161"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF616161"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF616161"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -827,64 +862,367 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AC01BA1-7E02-4B9A-B53C-B29C9722552F}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="A1:F1"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="36.26953125" customWidth="1"/>
+    <col min="2" max="2" width="12.08984375" customWidth="1"/>
     <col min="3" max="3" width="30.26953125" customWidth="1"/>
     <col min="4" max="4" width="25.54296875" customWidth="1"/>
     <col min="5" max="5" width="15.54296875" customWidth="1"/>
     <col min="6" max="6" width="37.7265625" customWidth="1"/>
+    <col min="10" max="10" width="13.1796875" customWidth="1"/>
+    <col min="11" max="11" width="15.7265625" customWidth="1"/>
+    <col min="14" max="14" width="13.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:14" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="L1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="M1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="N1" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <v>7349017534</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2">
+        <v>7349017534</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>7349017534</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3">
+        <v>7349017534</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8">
+        <v>9731749971</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" t="s">
+        <v>34</v>
+      </c>
+      <c r="J16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A29" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+    </row>
+    <row r="30" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B30" s="3"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="L30" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="M30" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="N30" s="3" t="s">
         <v>45</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" tooltip="mailto:supriya@36" display="mailto:supriya@36" xr:uid="{1B13A03D-8BC4-41AA-91A4-F03A00E03031}"/>
+    <hyperlink ref="K30" r:id="rId1" tooltip="mailto:supriya@36" display="mailto:supriya@36" xr:uid="{AA22EAD0-99EF-437D-A72E-727A56CC510F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -892,12 +1230,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100066650AE11F9D94F9BEC415F2F7F71AC" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="39d218c5b218fd11c7b1e015428ba1b0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8f0c852b-215b-4ad8-8d40-2e4064e0668d" xmlns:ns4="9c6c6072-304f-419a-b7e8-c670f973c5eb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e32445469b0a8b73f6a34ac0168539e2" ns3:_="" ns4:_="">
     <xsd:import namespace="8f0c852b-215b-4ad8-8d40-2e4064e0668d"/>
@@ -1094,6 +1426,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1104,23 +1442,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC7F54BF-14C3-4105-920F-7FCBFFA7E40D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="8f0c852b-215b-4ad8-8d40-2e4064e0668d"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="9c6c6072-304f-419a-b7e8-c670f973c5eb"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9838879D-783C-41A7-8468-DC0782555013}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1139,6 +1460,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC7F54BF-14C3-4105-920F-7FCBFFA7E40D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="8f0c852b-215b-4ad8-8d40-2e4064e0668d"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="9c6c6072-304f-419a-b7e8-c670f973c5eb"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5040F04D-8C74-4CDD-9A06-087701F18320}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Added Log4j and TestCases
</commit_message>
<xml_diff>
--- a/resources/DATAFILE.xlsx
+++ b/resources/DATAFILE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My Learning\Framework\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5102854C-E6AD-4780-95C4-928A409F695C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDE5E161-BD4E-4EA8-9C44-52EE8011D5FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{5F3B00A6-1F83-4E01-BEDD-A24AF5294CA6}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5F3B00A6-1F83-4E01-BEDD-A24AF5294CA6}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA_FILE" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="50">
   <si>
     <t>TC_NAME</t>
   </si>
@@ -142,9 +142,6 @@
     <t>Powerbank</t>
   </si>
   <si>
-    <t>TC_002_AMAZON_LOGIN</t>
-  </si>
-  <si>
     <t>JOB</t>
   </si>
   <si>
@@ -175,46 +172,19 @@
     <t>Bengaluru</t>
   </si>
   <si>
-    <t>TC_002_LOGIN_TEST</t>
-  </si>
-  <si>
-    <t>TC_001_LOGIN_TEST_1</t>
-  </si>
-  <si>
-    <t>TC_002_LOGIN_TEST_2</t>
-  </si>
-  <si>
-    <t>TC_003_LOGIN_TEST_3</t>
-  </si>
-  <si>
-    <t>TC_002_HOMEPAGE_TEST_2</t>
-  </si>
-  <si>
-    <t>TC_003_HOMEPAGE_TEST_3</t>
-  </si>
-  <si>
-    <t>TC_001_INVENTORY_TEST_1</t>
-  </si>
-  <si>
-    <t>Edge</t>
-  </si>
-  <si>
-    <t>TC_002_INVENTORY_TEST_2</t>
-  </si>
-  <si>
-    <t>TC_003_INVENTORY_TEST_3</t>
-  </si>
-  <si>
-    <t>TC_002_HOMEPAGE_TEST_1</t>
-  </si>
-  <si>
-    <t>TC_002_HOMEPAGE_TEST_3</t>
-  </si>
-  <si>
-    <t>TC_002_HOMEPAGE_TEST_4</t>
-  </si>
-  <si>
-    <t>TC_002_HOMEPAGE_TEST_5</t>
+    <t>TC_002_VERIFY_HOMEPAGE</t>
+  </si>
+  <si>
+    <t>TC_001_LOGIN</t>
+  </si>
+  <si>
+    <t>TC_003_AMAZON_SEARCH ITEM</t>
+  </si>
+  <si>
+    <t>TC_004_AMAZON_ADD TO CART</t>
+  </si>
+  <si>
+    <t>TC_005_PROCEED_TO_BUY</t>
   </si>
 </sst>
 </file>
@@ -246,7 +216,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -255,7 +224,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -293,10 +262,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -614,10 +581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D199509-3F83-478C-9D52-DA2EDFB81A9C}">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -667,7 +634,7 @@
       </c>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -692,7 +659,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -708,86 +675,88 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="A4" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
         <v>16</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J5" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
-      </c>
-      <c r="C8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H8">
-        <v>9731749971</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9">
+        <v>9731749971</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -795,7 +764,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -803,7 +772,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
@@ -811,7 +780,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
@@ -819,7 +788,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B14" t="s">
         <v>11</v>
@@ -827,7 +796,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B15" t="s">
         <v>11</v>
@@ -835,16 +804,48 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>33</v>
       </c>
-      <c r="B16" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" t="s">
         <v>34</v>
       </c>
-      <c r="J16" t="s">
+      <c r="J17" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A18" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A19" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A20" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -853,7 +854,7 @@
     <hyperlink ref="D2" r:id="rId2" display="supriya@36" xr:uid="{5D0079A2-4C1E-426C-8B37-A9D4B2C72B13}"/>
     <hyperlink ref="D3" r:id="rId3" display="supriya@36" xr:uid="{CBE5670A-1746-4C31-B317-813BDB480B10}"/>
     <hyperlink ref="F3" r:id="rId4" xr:uid="{7A3C7113-C825-40E8-89C2-53BC619DC829}"/>
-    <hyperlink ref="F8" r:id="rId5" xr:uid="{C8825C07-7343-4E1C-8B52-02785D4157AE}"/>
+    <hyperlink ref="F9" r:id="rId5" xr:uid="{C8825C07-7343-4E1C-8B52-02785D4157AE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
@@ -862,367 +863,75 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AC01BA1-7E02-4B9A-B53C-B29C9722552F}">
-  <dimension ref="A1:N30"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="36.26953125" customWidth="1"/>
-    <col min="2" max="2" width="12.08984375" customWidth="1"/>
-    <col min="3" max="3" width="30.26953125" customWidth="1"/>
-    <col min="4" max="4" width="25.54296875" customWidth="1"/>
-    <col min="5" max="5" width="15.54296875" customWidth="1"/>
-    <col min="6" max="6" width="37.7265625" customWidth="1"/>
-    <col min="10" max="10" width="13.1796875" customWidth="1"/>
-    <col min="11" max="11" width="15.7265625" customWidth="1"/>
-    <col min="14" max="14" width="13.6328125" customWidth="1"/>
+    <col min="5" max="5" width="13.1796875" customWidth="1"/>
+    <col min="6" max="6" width="15.7265625" customWidth="1"/>
+    <col min="9" max="9" width="13.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="13" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="D1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="E1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="F1" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="H1" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="I1" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="N1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2">
-        <v>7349017534</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2">
-        <v>7349017534</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3">
-        <v>7349017534</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3">
-        <v>7349017534</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" t="s">
-        <v>20</v>
-      </c>
-      <c r="J6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" t="s">
-        <v>25</v>
-      </c>
-      <c r="H8">
-        <v>9731749971</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" t="s">
-        <v>34</v>
-      </c>
-      <c r="J16" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>52</v>
-      </c>
-      <c r="B22" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>56</v>
-      </c>
-      <c r="B25" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>50</v>
-      </c>
-      <c r="B26" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>57</v>
-      </c>
-      <c r="B27" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>58</v>
-      </c>
-      <c r="B28" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A29" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-    </row>
-    <row r="30" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="3" t="s">
+      <c r="B2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="3"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3" t="s">
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
-      <c r="K30" s="7" t="s">
+      <c r="G2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="L30" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="M30" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="N30" s="3" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K30" r:id="rId1" tooltip="mailto:supriya@36" display="mailto:supriya@36" xr:uid="{AA22EAD0-99EF-437D-A72E-727A56CC510F}"/>
+    <hyperlink ref="F2" r:id="rId1" tooltip="mailto:supriya@36" display="mailto:supriya@36" xr:uid="{AA22EAD0-99EF-437D-A72E-727A56CC510F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -1230,6 +939,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100066650AE11F9D94F9BEC415F2F7F71AC" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="39d218c5b218fd11c7b1e015428ba1b0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8f0c852b-215b-4ad8-8d40-2e4064e0668d" xmlns:ns4="9c6c6072-304f-419a-b7e8-c670f973c5eb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e32445469b0a8b73f6a34ac0168539e2" ns3:_="" ns4:_="">
     <xsd:import namespace="8f0c852b-215b-4ad8-8d40-2e4064e0668d"/>
@@ -1426,22 +1150,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC7F54BF-14C3-4105-920F-7FCBFFA7E40D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="8f0c852b-215b-4ad8-8d40-2e4064e0668d"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="9c6c6072-304f-419a-b7e8-c670f973c5eb"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5040F04D-8C74-4CDD-9A06-087701F18320}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9838879D-783C-41A7-8468-DC0782555013}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1458,29 +1192,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC7F54BF-14C3-4105-920F-7FCBFFA7E40D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="8f0c852b-215b-4ad8-8d40-2e4064e0668d"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="9c6c6072-304f-419a-b7e8-c670f973c5eb"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5040F04D-8C74-4CDD-9A06-087701F18320}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Modified Log4j and testcases
</commit_message>
<xml_diff>
--- a/resources/DATAFILE.xlsx
+++ b/resources/DATAFILE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My Learning\Framework\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDE5E161-BD4E-4EA8-9C44-52EE8011D5FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF9D70C3-C41F-48B8-8AF2-A8CC92EDB806}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5F3B00A6-1F83-4E01-BEDD-A24AF5294CA6}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
   <si>
     <t>TC_NAME</t>
   </si>
@@ -67,81 +67,9 @@
     <t>SEARCH ITEM</t>
   </si>
   <si>
-    <t>TC_001_CREATEACCOUNT_TEST</t>
-  </si>
-  <si>
     <t>Chrome</t>
   </si>
   <si>
-    <t>supriya4</t>
-  </si>
-  <si>
-    <t>supriya4@deloitte.com</t>
-  </si>
-  <si>
-    <t>supriya</t>
-  </si>
-  <si>
-    <t>TC_003_CART_TEST</t>
-  </si>
-  <si>
-    <t>Bag</t>
-  </si>
-  <si>
-    <t>TC_004_Search item_TEST</t>
-  </si>
-  <si>
-    <t>Furniture</t>
-  </si>
-  <si>
-    <t>TC_005_Wishlist_TEST</t>
-  </si>
-  <si>
-    <t>Book</t>
-  </si>
-  <si>
-    <t>TC_006_Remove item_TEST</t>
-  </si>
-  <si>
-    <t>TC_007_ADD ACCOUNT_TEST</t>
-  </si>
-  <si>
-    <t>Chaitra DB</t>
-  </si>
-  <si>
-    <t>Chaitra@1809</t>
-  </si>
-  <si>
-    <t>chaitradb018@gmail.com</t>
-  </si>
-  <si>
-    <t>TC_008_LOGOUT_TEST</t>
-  </si>
-  <si>
-    <t>TC_009_RETURNS AND ORDERS_TEST</t>
-  </si>
-  <si>
-    <t>TC_010_ORDERS_TEST</t>
-  </si>
-  <si>
-    <t>TC_011_BUY AGAIN_TEST</t>
-  </si>
-  <si>
-    <t>TC_012_NOT YET SHIPPED_TEST</t>
-  </si>
-  <si>
-    <t>TC_013_CANCELLED ORDERS_TEST</t>
-  </si>
-  <si>
-    <t>TC_013_TRACK PACKAGE_TEST</t>
-  </si>
-  <si>
-    <t>TC_013_SEARCH ORDERS_TEST</t>
-  </si>
-  <si>
-    <t>Powerbank</t>
-  </si>
-  <si>
     <t>JOB</t>
   </si>
   <si>
@@ -185,6 +113,15 @@
   </si>
   <si>
     <t>TC_005_PROCEED_TO_BUY</t>
+  </si>
+  <si>
+    <t>laptop</t>
+  </si>
+  <si>
+    <t>amrutadanawade18@gmail.com</t>
+  </si>
+  <si>
+    <t>Amruta_18;</t>
   </si>
 </sst>
 </file>
@@ -581,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D199509-3F83-478C-9D52-DA2EDFB81A9C}">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -596,12 +533,9 @@
     <col min="5" max="5" width="12.6328125" customWidth="1"/>
     <col min="6" max="6" width="23.08984375" customWidth="1"/>
     <col min="7" max="7" width="9.6328125" customWidth="1"/>
-    <col min="8" max="8" width="14" customWidth="1"/>
-    <col min="9" max="9" width="17.6328125" customWidth="1"/>
-    <col min="10" max="10" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -623,241 +557,78 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1"/>
-    </row>
-    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="2">
-        <v>7349017534</v>
+      <c r="D2" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2">
-        <v>7349017534</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>46</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="2">
-        <v>7349017534</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3">
-        <v>7349017534</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>15</v>
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>17</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" t="s">
-        <v>20</v>
-      </c>
-      <c r="J7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H9">
-        <v>9731749971</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" t="s">
-        <v>34</v>
-      </c>
-      <c r="J17" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A18" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A19" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B19" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A20" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B20" t="s">
-        <v>11</v>
-      </c>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F8" s="2"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" s="6"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" s="6"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{C27D8E83-F92B-4BE2-9B44-F83EE7847300}"/>
-    <hyperlink ref="D2" r:id="rId2" display="supriya@36" xr:uid="{5D0079A2-4C1E-426C-8B37-A9D4B2C72B13}"/>
-    <hyperlink ref="D3" r:id="rId3" display="supriya@36" xr:uid="{CBE5670A-1746-4C31-B317-813BDB480B10}"/>
-    <hyperlink ref="F3" r:id="rId4" xr:uid="{7A3C7113-C825-40E8-89C2-53BC619DC829}"/>
-    <hyperlink ref="F9" r:id="rId5" xr:uid="{C8825C07-7343-4E1C-8B52-02785D4157AE}"/>
+    <hyperlink ref="D2" r:id="rId1" display="supriya@36" xr:uid="{CBE5670A-1746-4C31-B317-813BDB480B10}"/>
+    <hyperlink ref="F2" r:id="rId2" xr:uid="{7A3C7113-C825-40E8-89C2-53BC619DC829}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -894,39 +665,39 @@
         <v>9</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="5" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented xmlHander and added logs to testcases
</commit_message>
<xml_diff>
--- a/resources/DATAFILE.xlsx
+++ b/resources/DATAFILE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My Learning\Framework\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF9D70C3-C41F-48B8-8AF2-A8CC92EDB806}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E483EB6-23D0-4660-9616-D385EBD6995B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5F3B00A6-1F83-4E01-BEDD-A24AF5294CA6}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
   <si>
     <t>TC_NAME</t>
   </si>
@@ -122,13 +122,16 @@
   </si>
   <si>
     <t>Amruta_18;</t>
+  </si>
+  <si>
+    <t>TC_0056fcwf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -166,6 +169,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -188,7 +198,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -203,6 +213,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -521,7 +532,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -529,7 +540,7 @@
     <col min="1" max="1" width="33.453125" customWidth="1"/>
     <col min="2" max="2" width="16.54296875" customWidth="1"/>
     <col min="3" max="3" width="14.6328125" customWidth="1"/>
-    <col min="4" max="4" width="16.08984375" customWidth="1"/>
+    <col min="4" max="4" width="19.1796875" customWidth="1"/>
     <col min="5" max="5" width="12.6328125" customWidth="1"/>
     <col min="6" max="6" width="23.08984375" customWidth="1"/>
     <col min="7" max="7" width="9.6328125" customWidth="1"/>
@@ -566,10 +577,10 @@
       <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="8" t="s">
         <v>27</v>
       </c>
     </row>
@@ -607,6 +618,14 @@
         <v>25</v>
       </c>
       <c r="B6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implemented HomePage TestScenario and added changes to BaseClass
</commit_message>
<xml_diff>
--- a/resources/DATAFILE.xlsx
+++ b/resources/DATAFILE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My Learning\Framework\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E483EB6-23D0-4660-9616-D385EBD6995B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF01C6D8-7352-43F0-B9D6-9FEDA4F7E79B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5F3B00A6-1F83-4E01-BEDD-A24AF5294CA6}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
   <si>
     <t>TC_NAME</t>
   </si>
@@ -82,9 +82,6 @@
     <t>CITY</t>
   </si>
   <si>
-    <t>TC_001_POST_SINGLE_USER</t>
-  </si>
-  <si>
     <t>Ak</t>
   </si>
   <si>
@@ -103,9 +100,6 @@
     <t>TC_002_VERIFY_HOMEPAGE</t>
   </si>
   <si>
-    <t>TC_001_LOGIN</t>
-  </si>
-  <si>
     <t>TC_003_AMAZON_SEARCH ITEM</t>
   </si>
   <si>
@@ -124,14 +118,35 @@
     <t>Amruta_18;</t>
   </si>
   <si>
-    <t>TC_0056fcwf</t>
+    <t>TC_API_002_POST_SINGLE_USER</t>
+  </si>
+  <si>
+    <t>Prakruthi123!</t>
+  </si>
+  <si>
+    <t>prakruthi.koteshwar@gmail.com</t>
+  </si>
+  <si>
+    <t>TC_001_LOGIN_Positive</t>
+  </si>
+  <si>
+    <t>TC_001_LOGIN_Negative</t>
+  </si>
+  <si>
+    <t>TC_007_CLICK_ON_ORDERS</t>
+  </si>
+  <si>
+    <t>TC_008_CLICK_ON_LANGUAGE_OPTIONS</t>
+  </si>
+  <si>
+    <t>TC_009_CLICK_ON_HELP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -151,13 +166,6 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -198,22 +206,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -532,17 +539,17 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="33.453125" customWidth="1"/>
+    <col min="1" max="1" width="36.54296875" customWidth="1"/>
     <col min="2" max="2" width="16.54296875" customWidth="1"/>
     <col min="3" max="3" width="14.6328125" customWidth="1"/>
     <col min="4" max="4" width="19.1796875" customWidth="1"/>
     <col min="5" max="5" width="12.6328125" customWidth="1"/>
-    <col min="6" max="6" width="23.08984375" customWidth="1"/>
+    <col min="6" max="6" width="26.1796875" customWidth="1"/>
     <col min="7" max="7" width="9.6328125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -571,83 +578,136 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
-        <v>22</v>
+      <c r="A2" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>27</v>
+      <c r="D2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="6" t="s">
-        <v>21</v>
+      <c r="A3" s="7" t="s">
+        <v>30</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="6" t="s">
-        <v>23</v>
+      <c r="D3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="E4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="6" t="s">
-        <v>24</v>
+      <c r="D4" s="2"/>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="6" t="s">
-        <v>25</v>
+      <c r="A6" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="6" t="s">
-        <v>29</v>
+      <c r="A7" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="F8" s="2"/>
+      <c r="A8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="3"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="3"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="3"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="3"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="3"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="3"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" s="6"/>
+      <c r="A17" s="3"/>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" s="6"/>
+      <c r="A18" s="3"/>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" s="6"/>
+      <c r="A19" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" display="supriya@36" xr:uid="{CBE5670A-1746-4C31-B317-813BDB480B10}"/>
     <hyperlink ref="F2" r:id="rId2" xr:uid="{7A3C7113-C825-40E8-89C2-53BC619DC829}"/>
+    <hyperlink ref="F3" r:id="rId3" xr:uid="{BA77B0C0-DB43-4D69-9533-051CC375B7A0}"/>
+    <hyperlink ref="F8" r:id="rId4" xr:uid="{933F36AB-1639-45C7-A5B5-3DBB787CDF03}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -656,7 +716,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -683,48 +743,42 @@
       <c r="E1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="F2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="5" t="s">
+      <c r="G2" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>20</v>
-      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" tooltip="mailto:supriya@36" display="mailto:supriya@36" xr:uid="{AA22EAD0-99EF-437D-A72E-727A56CC510F}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Adding updated RunnerFile and DataFile
</commit_message>
<xml_diff>
--- a/resources/DATAFILE.xlsx
+++ b/resources/DATAFILE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My Learning\Framework\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF01C6D8-7352-43F0-B9D6-9FEDA4F7E79B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4D3FB8E-2D50-4E9F-B635-C287E8941675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5F3B00A6-1F83-4E01-BEDD-A24AF5294CA6}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{5F3B00A6-1F83-4E01-BEDD-A24AF5294CA6}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA_FILE" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
   <si>
     <t>TC_NAME</t>
   </si>
@@ -137,9 +137,6 @@
   </si>
   <si>
     <t>TC_008_CLICK_ON_LANGUAGE_OPTIONS</t>
-  </si>
-  <si>
-    <t>TC_009_CLICK_ON_HELP</t>
   </si>
 </sst>
 </file>
@@ -536,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D199509-3F83-478C-9D52-DA2EDFB81A9C}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -665,12 +662,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
+      <c r="A10" s="3"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
@@ -695,9 +687,6 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -715,8 +704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AC01BA1-7E02-4B9A-B53C-B29C9722552F}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Added comments and modified API calls to read input data from file
</commit_message>
<xml_diff>
--- a/resources/DATAFILE.xlsx
+++ b/resources/DATAFILE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My Learning\Framework\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4D3FB8E-2D50-4E9F-B635-C287E8941675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24A7193D-DBCE-4228-B82A-D65A4047B723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{5F3B00A6-1F83-4E01-BEDD-A24AF5294CA6}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
   <si>
     <t>TC_NAME</t>
   </si>
@@ -58,15 +58,6 @@
     <t>NAME</t>
   </si>
   <si>
-    <t>MOBILE</t>
-  </si>
-  <si>
-    <t>ADDRESS</t>
-  </si>
-  <si>
-    <t>SEARCH ITEM</t>
-  </si>
-  <si>
     <t>Chrome</t>
   </si>
   <si>
@@ -82,9 +73,6 @@
     <t>CITY</t>
   </si>
   <si>
-    <t>Ak</t>
-  </si>
-  <si>
     <t>Developer</t>
   </si>
   <si>
@@ -137,6 +125,69 @@
   </si>
   <si>
     <t>TC_008_CLICK_ON_LANGUAGE_OPTIONS</t>
+  </si>
+  <si>
+    <t>/api/users/{id}</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>/api/users</t>
+  </si>
+  <si>
+    <t>UserId</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>page</t>
+  </si>
+  <si>
+    <t>ENDPOINT</t>
+  </si>
+  <si>
+    <t>PATH_KEY</t>
+  </si>
+  <si>
+    <t>PATH_VALUE</t>
+  </si>
+  <si>
+    <t>QUERY_KEY</t>
+  </si>
+  <si>
+    <t>QUERY_VALUE</t>
+  </si>
+  <si>
+    <t>AUTH_TOKEN</t>
+  </si>
+  <si>
+    <t>HEADER_KEY</t>
+  </si>
+  <si>
+    <t>HEADER_VALUE</t>
+  </si>
+  <si>
+    <t>TC_API_001_GET_CALL</t>
+  </si>
+  <si>
+    <t>TC_API_003_PUT_CALL</t>
+  </si>
+  <si>
+    <t>TC_API_004_DELETE_CALL</t>
+  </si>
+  <si>
+    <t>Rahul</t>
+  </si>
+  <si>
+    <t>Ganesh</t>
+  </si>
+  <si>
+    <t>QA</t>
+  </si>
+  <si>
+    <t>TC_API_005_GET_ALL_USER</t>
   </si>
 </sst>
 </file>
@@ -203,14 +254,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -536,7 +584,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -576,89 +624,89 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D4" s="2"/>
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
@@ -702,68 +750,176 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AC01BA1-7E02-4B9A-B53C-B29C9722552F}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="36.26953125" customWidth="1"/>
+    <col min="2" max="2" width="26.26953125" customWidth="1"/>
+    <col min="3" max="3" width="20.6328125" customWidth="1"/>
+    <col min="4" max="4" width="17.6328125" customWidth="1"/>
     <col min="5" max="5" width="13.1796875" customWidth="1"/>
     <col min="6" max="6" width="15.7265625" customWidth="1"/>
+    <col min="7" max="7" width="14.26953125" customWidth="1"/>
+    <col min="8" max="8" width="13.54296875" customWidth="1"/>
     <col min="9" max="9" width="13.6328125" customWidth="1"/>
+    <col min="10" max="10" width="10.81640625" customWidth="1"/>
+    <col min="11" max="11" width="13.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="M1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="4" t="s">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K3" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="L3" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="M3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="N3" t="s">
         <v>15</v>
       </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" t="s">
-        <v>19</v>
-      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="J4" t="s">
+        <v>48</v>
+      </c>
+      <c r="K4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="H5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A10" s="5"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A11" s="5"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A12" s="5"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A13" s="5"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A14" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -772,18 +928,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -984,6 +1140,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5040F04D-8C74-4CDD-9A06-087701F18320}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC7F54BF-14C3-4105-920F-7FCBFFA7E40D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
@@ -996,14 +1160,6 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5040F04D-8C74-4CDD-9A06-087701F18320}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Modified the test cases
</commit_message>
<xml_diff>
--- a/resources/DATAFILE.xlsx
+++ b/resources/DATAFILE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My Learning\Framework\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24A7193D-DBCE-4228-B82A-D65A4047B723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C363E7B-43B4-4D26-97C1-585362D0C483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{5F3B00A6-1F83-4E01-BEDD-A24AF5294CA6}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5F3B00A6-1F83-4E01-BEDD-A24AF5294CA6}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA_FILE" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="52">
   <si>
     <t>TC_NAME</t>
   </si>
@@ -188,6 +188,9 @@
   </si>
   <si>
     <t>TC_API_005_GET_ALL_USER</t>
+  </si>
+  <si>
+    <t>Prakruthi</t>
   </si>
 </sst>
 </file>
@@ -583,8 +586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D199509-3F83-478C-9D52-DA2EDFB81A9C}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -643,6 +646,9 @@
       <c r="B3" t="s">
         <v>7</v>
       </c>
+      <c r="C3" t="s">
+        <v>51</v>
+      </c>
       <c r="D3" s="4" t="s">
         <v>24</v>
       </c>
@@ -752,8 +758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AC01BA1-7E02-4B9A-B53C-B29C9722552F}">
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -928,21 +934,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100066650AE11F9D94F9BEC415F2F7F71AC" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="39d218c5b218fd11c7b1e015428ba1b0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8f0c852b-215b-4ad8-8d40-2e4064e0668d" xmlns:ns4="9c6c6072-304f-419a-b7e8-c670f973c5eb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e32445469b0a8b73f6a34ac0168539e2" ns3:_="" ns4:_="">
     <xsd:import namespace="8f0c852b-215b-4ad8-8d40-2e4064e0668d"/>
@@ -1139,10 +1130,36 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5040F04D-8C74-4CDD-9A06-087701F18320}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9838879D-783C-41A7-8468-DC0782555013}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8f0c852b-215b-4ad8-8d40-2e4064e0668d"/>
+    <ds:schemaRef ds:uri="9c6c6072-304f-419a-b7e8-c670f973c5eb"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1165,20 +1182,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9838879D-783C-41A7-8468-DC0782555013}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5040F04D-8C74-4CDD-9A06-087701F18320}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="8f0c852b-215b-4ad8-8d40-2e4064e0668d"/>
-    <ds:schemaRef ds:uri="9c6c6072-304f-419a-b7e8-c670f973c5eb"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Modified the test cases in Login Page
</commit_message>
<xml_diff>
--- a/resources/DATAFILE.xlsx
+++ b/resources/DATAFILE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My Learning\Framework\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C363E7B-43B4-4D26-97C1-585362D0C483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{612A637E-FEE8-4DB3-B707-BE185569CFFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5F3B00A6-1F83-4E01-BEDD-A24AF5294CA6}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
   <si>
     <t>TC_NAME</t>
   </si>
@@ -188,9 +188,6 @@
   </si>
   <si>
     <t>TC_API_005_GET_ALL_USER</t>
-  </si>
-  <si>
-    <t>Prakruthi</t>
   </si>
 </sst>
 </file>
@@ -646,9 +643,6 @@
       <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>51</v>
-      </c>
       <c r="D3" s="4" t="s">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
Modified testcases and listenerclass
</commit_message>
<xml_diff>
--- a/resources/DATAFILE.xlsx
+++ b/resources/DATAFILE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My Learning\Framework\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{612A637E-FEE8-4DB3-B707-BE185569CFFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A702774-22C3-4C61-8535-5787D0DDBB18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5F3B00A6-1F83-4E01-BEDD-A24AF5294CA6}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="55">
   <si>
     <t>TC_NAME</t>
   </si>
@@ -188,6 +188,18 @@
   </si>
   <si>
     <t>TC_API_005_GET_ALL_USER</t>
+  </si>
+  <si>
+    <t>TC_009_GO_TO_HELP_PAGE</t>
+  </si>
+  <si>
+    <t>TC_010_Go_TO_CONTACT_US_PAGE</t>
+  </si>
+  <si>
+    <t>TC_011_CHANGE_COUNTRY</t>
+  </si>
+  <si>
+    <t>TC_012_ADD_NEW_ADDRESS_PAGE</t>
   </si>
 </sst>
 </file>
@@ -581,10 +593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D199509-3F83-478C-9D52-DA2EDFB81A9C}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -678,6 +690,9 @@
       <c r="B6" t="s">
         <v>7</v>
       </c>
+      <c r="E6" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
@@ -686,6 +701,9 @@
       <c r="B7" t="s">
         <v>7</v>
       </c>
+      <c r="E7" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
@@ -694,7 +712,7 @@
       <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="4" t="s">
         <v>24</v>
       </c>
       <c r="F8" s="2" t="s">
@@ -710,16 +728,48 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="3"/>
+      <c r="A10" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="3"/>
+      <c r="A11" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="3"/>
+      <c r="A12" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="3"/>
+      <c r="A13" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
@@ -732,19 +782,18 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" display="supriya@36" xr:uid="{CBE5670A-1746-4C31-B317-813BDB480B10}"/>
     <hyperlink ref="F2" r:id="rId2" xr:uid="{7A3C7113-C825-40E8-89C2-53BC619DC829}"/>
     <hyperlink ref="F3" r:id="rId3" xr:uid="{BA77B0C0-DB43-4D69-9533-051CC375B7A0}"/>
-    <hyperlink ref="F8" r:id="rId4" xr:uid="{933F36AB-1639-45C7-A5B5-3DBB787CDF03}"/>
+    <hyperlink ref="F11" r:id="rId4" xr:uid="{399FEB8C-0D53-4A1E-9ECC-516C5DCCD838}"/>
+    <hyperlink ref="F13" r:id="rId5" xr:uid="{96CB7B94-9CCB-49C6-9131-FFEC1038C8E3}"/>
+    <hyperlink ref="F8" r:id="rId6" xr:uid="{17E70DA2-7A34-49D8-ABED-191B2B9AA561}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -928,6 +977,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100066650AE11F9D94F9BEC415F2F7F71AC" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="39d218c5b218fd11c7b1e015428ba1b0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8f0c852b-215b-4ad8-8d40-2e4064e0668d" xmlns:ns4="9c6c6072-304f-419a-b7e8-c670f973c5eb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e32445469b0a8b73f6a34ac0168539e2" ns3:_="" ns4:_="">
     <xsd:import namespace="8f0c852b-215b-4ad8-8d40-2e4064e0668d"/>
@@ -1124,22 +1182,21 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5040F04D-8C74-4CDD-9A06-087701F18320}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9838879D-783C-41A7-8468-DC0782555013}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1158,7 +1215,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC7F54BF-14C3-4105-920F-7FCBFFA7E40D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
@@ -1173,12 +1230,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5040F04D-8C74-4CDD-9A06-087701F18320}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Modified testcases and utility classes
</commit_message>
<xml_diff>
--- a/resources/DATAFILE.xlsx
+++ b/resources/DATAFILE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My Learning\Framework\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A702774-22C3-4C61-8535-5787D0DDBB18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{165CF90F-2827-4F61-810B-5DF65A681F0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5F3B00A6-1F83-4E01-BEDD-A24AF5294CA6}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="58">
   <si>
     <t>TC_NAME</t>
   </si>
@@ -200,6 +200,15 @@
   </si>
   <si>
     <t>TC_012_ADD_NEW_ADDRESS_PAGE</t>
+  </si>
+  <si>
+    <t>Edge</t>
+  </si>
+  <si>
+    <t>mobile</t>
+  </si>
+  <si>
+    <t>TC_013_GO_TO_NEW_RELEASE_PAGE</t>
   </si>
 </sst>
 </file>
@@ -593,10 +602,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D199509-3F83-478C-9D52-DA2EDFB81A9C}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -666,9 +675,6 @@
       <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
       <c r="D4" s="2"/>
       <c r="F4" s="2"/>
     </row>
@@ -683,23 +689,23 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>55</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>55</v>
       </c>
       <c r="E7" t="s">
         <v>20</v>
@@ -707,93 +713,111 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>25</v>
+      <c r="E8" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
       </c>
+      <c r="D9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
       </c>
+      <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
       </c>
+      <c r="D12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D14" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="3"/>
-    </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="3"/>
+      <c r="A15" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" display="supriya@36" xr:uid="{CBE5670A-1746-4C31-B317-813BDB480B10}"/>
     <hyperlink ref="F2" r:id="rId2" xr:uid="{7A3C7113-C825-40E8-89C2-53BC619DC829}"/>
-    <hyperlink ref="F3" r:id="rId3" xr:uid="{BA77B0C0-DB43-4D69-9533-051CC375B7A0}"/>
-    <hyperlink ref="F11" r:id="rId4" xr:uid="{399FEB8C-0D53-4A1E-9ECC-516C5DCCD838}"/>
-    <hyperlink ref="F13" r:id="rId5" xr:uid="{96CB7B94-9CCB-49C6-9131-FFEC1038C8E3}"/>
-    <hyperlink ref="F8" r:id="rId6" xr:uid="{17E70DA2-7A34-49D8-ABED-191B2B9AA561}"/>
+    <hyperlink ref="F12" r:id="rId3" xr:uid="{399FEB8C-0D53-4A1E-9ECC-516C5DCCD838}"/>
+    <hyperlink ref="F14" r:id="rId4" xr:uid="{96CB7B94-9CCB-49C6-9131-FFEC1038C8E3}"/>
+    <hyperlink ref="F9" r:id="rId5" xr:uid="{17E70DA2-7A34-49D8-ABED-191B2B9AA561}"/>
+    <hyperlink ref="D3" r:id="rId6" display="supriya@36" xr:uid="{A0A00EAF-875C-43C4-89AB-9A855206069A}"/>
+    <hyperlink ref="F3" r:id="rId7" xr:uid="{0CF0B231-01C1-4C39-BB92-9C511B687C4D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 
@@ -802,7 +826,7 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -977,6 +1001,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -985,7 +1015,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100066650AE11F9D94F9BEC415F2F7F71AC" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="39d218c5b218fd11c7b1e015428ba1b0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8f0c852b-215b-4ad8-8d40-2e4064e0668d" xmlns:ns4="9c6c6072-304f-419a-b7e8-c670f973c5eb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e32445469b0a8b73f6a34ac0168539e2" ns3:_="" ns4:_="">
     <xsd:import namespace="8f0c852b-215b-4ad8-8d40-2e4064e0668d"/>
@@ -1182,13 +1212,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC7F54BF-14C3-4105-920F-7FCBFFA7E40D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="8f0c852b-215b-4ad8-8d40-2e4064e0668d"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="9c6c6072-304f-419a-b7e8-c670f973c5eb"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5040F04D-8C74-4CDD-9A06-087701F18320}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -1196,7 +1237,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9838879D-783C-41A7-8468-DC0782555013}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1213,21 +1254,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC7F54BF-14C3-4105-920F-7FCBFFA7E40D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="8f0c852b-215b-4ad8-8d40-2e4064e0668d"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="9c6c6072-304f-419a-b7e8-c670f973c5eb"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>